<commit_message>
Update T3 Experiment Interaction Tracking.xlsx
</commit_message>
<xml_diff>
--- a/Experement Build/Test 3/T3 Experiment Interaction Tracking.xlsx
+++ b/Experement Build/Test 3/T3 Experiment Interaction Tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Llama\GitHub\Blockchain-Voting-System\Experement Build\Test 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1359E506-CB3E-4BA3-A7AE-1508239E0975}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FFFDE18-C336-4FEC-AFEF-6364F6334AC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -558,12 +558,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -571,12 +565,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -595,6 +583,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -920,7 +920,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I131" sqref="I131"/>
+      <selection pane="bottomLeft" activeCell="I60" sqref="I60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -940,51 +940,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="42" x14ac:dyDescent="0.35">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="I1" s="20" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18" t="s">
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="18"/>
-      <c r="I2" s="24"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="30"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="25">
+      <c r="A3" s="21">
         <v>1</v>
       </c>
       <c r="B3" s="1">
@@ -1013,7 +1013,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="25">
+      <c r="A4" s="21">
         <v>2</v>
       </c>
       <c r="B4" s="1">
@@ -1042,7 +1042,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="25">
+      <c r="A5" s="21">
         <v>3</v>
       </c>
       <c r="B5" s="1">
@@ -1071,7 +1071,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="25">
+      <c r="A6" s="21">
         <v>4</v>
       </c>
       <c r="B6" s="1">
@@ -1100,7 +1100,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="25">
+      <c r="A7" s="21">
         <v>5</v>
       </c>
       <c r="B7" s="1">
@@ -1129,7 +1129,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="25">
+      <c r="A8" s="21">
         <v>6</v>
       </c>
       <c r="B8" s="1">
@@ -1158,7 +1158,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="25">
+      <c r="A9" s="21">
         <v>7</v>
       </c>
       <c r="B9" s="1">
@@ -1187,7 +1187,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="25">
+      <c r="A10" s="21">
         <v>8</v>
       </c>
       <c r="B10" s="1">
@@ -1216,7 +1216,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="25">
+      <c r="A11" s="21">
         <v>9</v>
       </c>
       <c r="B11" s="1">
@@ -1245,7 +1245,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="25">
+      <c r="A12" s="21">
         <v>10</v>
       </c>
       <c r="B12" s="1">
@@ -1274,22 +1274,22 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A13" s="23" t="s">
+      <c r="A13" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18" t="s">
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="H13" s="18"/>
-      <c r="I13" s="24"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="30"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" s="26">
+      <c r="A14" s="22">
         <v>11</v>
       </c>
       <c r="B14" s="3">
@@ -1319,7 +1319,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" s="26">
+      <c r="A15" s="22">
         <v>12</v>
       </c>
       <c r="B15" s="3">
@@ -1335,7 +1335,7 @@
         <v>16</v>
       </c>
       <c r="F15" s="3" t="str">
-        <f t="shared" ref="F15:F26" si="0">$F$12</f>
+        <f t="shared" ref="F15:F24" si="0">$F$12</f>
         <v>N/A</v>
       </c>
       <c r="G15" s="3" t="s">
@@ -1349,7 +1349,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" s="26">
+      <c r="A16" s="22">
         <v>13</v>
       </c>
       <c r="B16" s="3">
@@ -1379,7 +1379,7 @@
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A17" s="26">
+      <c r="A17" s="22">
         <v>14</v>
       </c>
       <c r="B17" s="3">
@@ -1409,7 +1409,7 @@
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A18" s="26">
+      <c r="A18" s="22">
         <v>15</v>
       </c>
       <c r="B18" s="3">
@@ -1439,7 +1439,7 @@
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A19" s="26">
+      <c r="A19" s="22">
         <v>16</v>
       </c>
       <c r="B19" s="3">
@@ -1469,7 +1469,7 @@
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A20" s="26">
+      <c r="A20" s="22">
         <v>17</v>
       </c>
       <c r="B20" s="3">
@@ -1499,7 +1499,7 @@
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A21" s="26">
+      <c r="A21" s="22">
         <v>18</v>
       </c>
       <c r="B21" s="3">
@@ -1529,7 +1529,7 @@
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A22" s="26">
+      <c r="A22" s="22">
         <v>19</v>
       </c>
       <c r="B22" s="3">
@@ -1571,7 +1571,7 @@
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A23" s="26">
+      <c r="A23" s="22">
         <v>20</v>
       </c>
       <c r="B23" s="3">
@@ -1601,7 +1601,7 @@
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A24" s="26">
+      <c r="A24" s="22">
         <v>21</v>
       </c>
       <c r="B24" s="3">
@@ -1631,22 +1631,22 @@
       </c>
     </row>
     <row r="25" spans="1:15" ht="21" x14ac:dyDescent="0.35">
-      <c r="A25" s="23" t="s">
+      <c r="A25" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="18"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18" t="s">
+      <c r="B25" s="29"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="H25" s="18"/>
-      <c r="I25" s="24"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="30"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A26" s="26">
+      <c r="A26" s="22">
         <v>22</v>
       </c>
       <c r="B26" s="5">
@@ -1675,7 +1675,7 @@
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A27" s="26">
+      <c r="A27" s="22">
         <v>23</v>
       </c>
       <c r="B27" s="5">
@@ -1704,7 +1704,7 @@
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A28" s="26">
+      <c r="A28" s="22">
         <v>24</v>
       </c>
       <c r="B28" s="5">
@@ -1733,7 +1733,7 @@
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A29" s="26">
+      <c r="A29" s="22">
         <v>25</v>
       </c>
       <c r="B29" s="5">
@@ -1762,7 +1762,7 @@
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A30" s="26">
+      <c r="A30" s="22">
         <v>26</v>
       </c>
       <c r="B30" s="5">
@@ -1791,7 +1791,7 @@
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A31" s="26">
+      <c r="A31" s="22">
         <v>27</v>
       </c>
       <c r="B31" s="5">
@@ -1820,7 +1820,7 @@
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A32" s="26">
+      <c r="A32" s="22">
         <v>28</v>
       </c>
       <c r="B32" s="5">
@@ -1849,7 +1849,7 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A33" s="26">
+      <c r="A33" s="22">
         <v>29</v>
       </c>
       <c r="B33" s="5">
@@ -1878,22 +1878,22 @@
       </c>
     </row>
     <row r="34" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A34" s="23" t="s">
+      <c r="A34" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18" t="s">
+      <c r="B34" s="29"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="29"/>
+      <c r="G34" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="H34" s="18"/>
-      <c r="I34" s="24"/>
+      <c r="H34" s="29"/>
+      <c r="I34" s="30"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A35" s="26">
+      <c r="A35" s="22">
         <v>30</v>
       </c>
       <c r="B35" s="6">
@@ -1922,7 +1922,7 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A36" s="26">
+      <c r="A36" s="22">
         <v>31</v>
       </c>
       <c r="B36" s="6">
@@ -1951,7 +1951,7 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A37" s="26">
+      <c r="A37" s="22">
         <v>32</v>
       </c>
       <c r="B37" s="6">
@@ -1980,7 +1980,7 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A38" s="26">
+      <c r="A38" s="22">
         <v>33</v>
       </c>
       <c r="B38" s="6">
@@ -2009,7 +2009,7 @@
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A39" s="26">
+      <c r="A39" s="22">
         <v>34</v>
       </c>
       <c r="B39" s="6">
@@ -2038,7 +2038,7 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A40" s="26">
+      <c r="A40" s="22">
         <v>35</v>
       </c>
       <c r="B40" s="6">
@@ -2067,7 +2067,7 @@
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A41" s="26">
+      <c r="A41" s="22">
         <v>36</v>
       </c>
       <c r="B41" s="6">
@@ -2096,7 +2096,7 @@
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A42" s="26">
+      <c r="A42" s="22">
         <v>37</v>
       </c>
       <c r="B42" s="6">
@@ -2125,7 +2125,7 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A43" s="26">
+      <c r="A43" s="22">
         <v>38</v>
       </c>
       <c r="B43" s="6">
@@ -2154,7 +2154,7 @@
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A44" s="26">
+      <c r="A44" s="22">
         <v>39</v>
       </c>
       <c r="B44" s="6">
@@ -2183,7 +2183,7 @@
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A45" s="26">
+      <c r="A45" s="22">
         <v>40</v>
       </c>
       <c r="B45" s="6">
@@ -2212,7 +2212,7 @@
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A46" s="26">
+      <c r="A46" s="22">
         <v>41</v>
       </c>
       <c r="B46" s="6">
@@ -2241,22 +2241,22 @@
       </c>
     </row>
     <row r="47" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A47" s="23" t="s">
+      <c r="A47" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="B47" s="18"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="18"/>
-      <c r="F47" s="18"/>
-      <c r="G47" s="18" t="s">
+      <c r="B47" s="29"/>
+      <c r="C47" s="29"/>
+      <c r="D47" s="29"/>
+      <c r="E47" s="29"/>
+      <c r="F47" s="29"/>
+      <c r="G47" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="H47" s="18"/>
-      <c r="I47" s="24"/>
+      <c r="H47" s="29"/>
+      <c r="I47" s="30"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A48" s="26">
+      <c r="A48" s="22">
         <v>42</v>
       </c>
       <c r="B48" s="7">
@@ -2285,7 +2285,7 @@
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A49" s="26">
+      <c r="A49" s="22">
         <v>43</v>
       </c>
       <c r="B49" s="7">
@@ -2314,7 +2314,7 @@
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A50" s="26">
+      <c r="A50" s="22">
         <v>44</v>
       </c>
       <c r="B50" s="7">
@@ -2343,7 +2343,7 @@
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A51" s="26">
+      <c r="A51" s="22">
         <v>45</v>
       </c>
       <c r="B51" s="7">
@@ -2372,7 +2372,7 @@
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A52" s="26">
+      <c r="A52" s="22">
         <v>46</v>
       </c>
       <c r="B52" s="7">
@@ -2401,7 +2401,7 @@
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A53" s="26">
+      <c r="A53" s="22">
         <v>47</v>
       </c>
       <c r="B53" s="7">
@@ -2430,7 +2430,7 @@
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A54" s="26">
+      <c r="A54" s="22">
         <v>48</v>
       </c>
       <c r="B54" s="7">
@@ -2459,7 +2459,7 @@
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A55" s="26">
+      <c r="A55" s="22">
         <v>49</v>
       </c>
       <c r="B55" s="7">
@@ -2487,7 +2487,7 @@
       <c r="M55" s="8"/>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A56" s="26">
+      <c r="A56" s="22">
         <v>50</v>
       </c>
       <c r="B56" s="7">
@@ -2516,7 +2516,7 @@
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A57" s="26">
+      <c r="A57" s="22">
         <v>51</v>
       </c>
       <c r="B57" s="7">
@@ -2545,7 +2545,7 @@
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A58" s="26">
+      <c r="A58" s="22">
         <v>52</v>
       </c>
       <c r="B58" s="7">
@@ -2574,22 +2574,22 @@
       </c>
     </row>
     <row r="59" spans="1:13" ht="21" x14ac:dyDescent="0.35">
-      <c r="A59" s="23" t="s">
+      <c r="A59" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="B59" s="18"/>
-      <c r="C59" s="18"/>
-      <c r="D59" s="18"/>
-      <c r="E59" s="18"/>
-      <c r="F59" s="18"/>
-      <c r="G59" s="18" t="s">
+      <c r="B59" s="29"/>
+      <c r="C59" s="29"/>
+      <c r="D59" s="29"/>
+      <c r="E59" s="29"/>
+      <c r="F59" s="29"/>
+      <c r="G59" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="H59" s="18"/>
-      <c r="I59" s="24"/>
+      <c r="H59" s="29"/>
+      <c r="I59" s="30"/>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A60" s="26">
+      <c r="A60" s="22">
         <v>53</v>
       </c>
       <c r="B60" s="9">
@@ -2618,7 +2618,7 @@
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A61" s="26">
+      <c r="A61" s="22">
         <v>54</v>
       </c>
       <c r="B61" s="9">
@@ -2647,7 +2647,7 @@
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A62" s="26">
+      <c r="A62" s="22">
         <v>55</v>
       </c>
       <c r="B62" s="9">
@@ -2676,7 +2676,7 @@
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A63" s="26">
+      <c r="A63" s="22">
         <v>56</v>
       </c>
       <c r="B63" s="9">
@@ -2705,7 +2705,7 @@
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A64" s="26">
+      <c r="A64" s="22">
         <v>57</v>
       </c>
       <c r="B64" s="9">
@@ -2734,7 +2734,7 @@
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A65" s="26">
+      <c r="A65" s="22">
         <v>58</v>
       </c>
       <c r="B65" s="9">
@@ -2763,7 +2763,7 @@
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A66" s="26">
+      <c r="A66" s="22">
         <v>59</v>
       </c>
       <c r="B66" s="9">
@@ -2792,7 +2792,7 @@
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A67" s="26">
+      <c r="A67" s="22">
         <v>60</v>
       </c>
       <c r="B67" s="9">
@@ -2821,22 +2821,22 @@
       </c>
     </row>
     <row r="68" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A68" s="23" t="s">
+      <c r="A68" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="B68" s="18"/>
-      <c r="C68" s="18"/>
-      <c r="D68" s="18"/>
-      <c r="E68" s="18"/>
-      <c r="F68" s="18"/>
-      <c r="G68" s="18" t="s">
+      <c r="B68" s="29"/>
+      <c r="C68" s="29"/>
+      <c r="D68" s="29"/>
+      <c r="E68" s="29"/>
+      <c r="F68" s="29"/>
+      <c r="G68" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="H68" s="18"/>
-      <c r="I68" s="24"/>
+      <c r="H68" s="29"/>
+      <c r="I68" s="30"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A69" s="26">
+      <c r="A69" s="22">
         <v>61</v>
       </c>
       <c r="B69" s="10">
@@ -2865,7 +2865,7 @@
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A70" s="26">
+      <c r="A70" s="22">
         <v>62</v>
       </c>
       <c r="B70" s="10">
@@ -2894,7 +2894,7 @@
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A71" s="26">
+      <c r="A71" s="22">
         <v>63</v>
       </c>
       <c r="B71" s="10">
@@ -2923,7 +2923,7 @@
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A72" s="26">
+      <c r="A72" s="22">
         <v>64</v>
       </c>
       <c r="B72" s="10">
@@ -2952,7 +2952,7 @@
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A73" s="26">
+      <c r="A73" s="22">
         <v>65</v>
       </c>
       <c r="B73" s="10">
@@ -2979,7 +2979,7 @@
       <c r="I73" s="2"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A74" s="26">
+      <c r="A74" s="22">
         <v>66</v>
       </c>
       <c r="B74" s="10">
@@ -3008,7 +3008,7 @@
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A75" s="26">
+      <c r="A75" s="22">
         <v>67</v>
       </c>
       <c r="B75" s="10">
@@ -3037,7 +3037,7 @@
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A76" s="26">
+      <c r="A76" s="22">
         <v>68</v>
       </c>
       <c r="B76" s="10">
@@ -3066,7 +3066,7 @@
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A77" s="26">
+      <c r="A77" s="22">
         <v>69</v>
       </c>
       <c r="B77" s="10">
@@ -3095,7 +3095,7 @@
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A78" s="26">
+      <c r="A78" s="22">
         <v>70</v>
       </c>
       <c r="B78" s="10">
@@ -3124,22 +3124,22 @@
       </c>
     </row>
     <row r="79" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A79" s="23" t="s">
+      <c r="A79" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="B79" s="18"/>
-      <c r="C79" s="18"/>
-      <c r="D79" s="18"/>
-      <c r="E79" s="18"/>
-      <c r="F79" s="18"/>
-      <c r="G79" s="18" t="s">
+      <c r="B79" s="29"/>
+      <c r="C79" s="29"/>
+      <c r="D79" s="29"/>
+      <c r="E79" s="29"/>
+      <c r="F79" s="29"/>
+      <c r="G79" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="H79" s="18"/>
-      <c r="I79" s="24"/>
+      <c r="H79" s="29"/>
+      <c r="I79" s="30"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A80" s="26">
+      <c r="A80" s="22">
         <v>71</v>
       </c>
       <c r="B80" s="11">
@@ -3168,7 +3168,7 @@
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A81" s="26">
+      <c r="A81" s="22">
         <v>72</v>
       </c>
       <c r="B81" s="11">
@@ -3197,7 +3197,7 @@
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A82" s="26">
+      <c r="A82" s="22">
         <v>73</v>
       </c>
       <c r="B82" s="11">
@@ -3226,7 +3226,7 @@
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A83" s="26">
+      <c r="A83" s="22">
         <v>74</v>
       </c>
       <c r="B83" s="11">
@@ -3255,7 +3255,7 @@
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A84" s="26">
+      <c r="A84" s="22">
         <v>75</v>
       </c>
       <c r="B84" s="11">
@@ -3282,7 +3282,7 @@
       <c r="I84" s="2"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A85" s="26">
+      <c r="A85" s="22">
         <v>76</v>
       </c>
       <c r="B85" s="11">
@@ -3311,7 +3311,7 @@
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A86" s="26">
+      <c r="A86" s="22">
         <v>77</v>
       </c>
       <c r="B86" s="11">
@@ -3340,7 +3340,7 @@
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A87" s="26">
+      <c r="A87" s="22">
         <v>78</v>
       </c>
       <c r="B87" s="11">
@@ -3369,7 +3369,7 @@
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A88" s="26">
+      <c r="A88" s="22">
         <v>79</v>
       </c>
       <c r="B88" s="11">
@@ -3398,7 +3398,7 @@
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A89" s="26">
+      <c r="A89" s="22">
         <v>80</v>
       </c>
       <c r="B89" s="11">
@@ -3427,22 +3427,22 @@
       </c>
     </row>
     <row r="90" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A90" s="23" t="s">
+      <c r="A90" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="B90" s="18"/>
-      <c r="C90" s="18"/>
-      <c r="D90" s="18"/>
-      <c r="E90" s="18"/>
-      <c r="F90" s="18"/>
-      <c r="G90" s="18" t="s">
+      <c r="B90" s="29"/>
+      <c r="C90" s="29"/>
+      <c r="D90" s="29"/>
+      <c r="E90" s="29"/>
+      <c r="F90" s="29"/>
+      <c r="G90" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="H90" s="18"/>
-      <c r="I90" s="24"/>
+      <c r="H90" s="29"/>
+      <c r="I90" s="30"/>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A91" s="26">
+      <c r="A91" s="22">
         <v>81</v>
       </c>
       <c r="B91" s="12">
@@ -3471,7 +3471,7 @@
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A92" s="26">
+      <c r="A92" s="22">
         <v>82</v>
       </c>
       <c r="B92" s="12">
@@ -3500,7 +3500,7 @@
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A93" s="26">
+      <c r="A93" s="22">
         <v>83</v>
       </c>
       <c r="B93" s="12">
@@ -3529,7 +3529,7 @@
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A94" s="26">
+      <c r="A94" s="22">
         <v>84</v>
       </c>
       <c r="B94" s="12">
@@ -3558,7 +3558,7 @@
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A95" s="26">
+      <c r="A95" s="22">
         <v>85</v>
       </c>
       <c r="B95" s="12">
@@ -3587,7 +3587,7 @@
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A96" s="26">
+      <c r="A96" s="22">
         <v>86</v>
       </c>
       <c r="B96" s="12">
@@ -3616,7 +3616,7 @@
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A97" s="26">
+      <c r="A97" s="22">
         <v>87</v>
       </c>
       <c r="B97" s="12">
@@ -3645,7 +3645,7 @@
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A98" s="26">
+      <c r="A98" s="22">
         <v>88</v>
       </c>
       <c r="B98" s="12">
@@ -3674,7 +3674,7 @@
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A99" s="26">
+      <c r="A99" s="22">
         <v>89</v>
       </c>
       <c r="B99" s="12">
@@ -3703,7 +3703,7 @@
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A100" s="26">
+      <c r="A100" s="22">
         <v>90</v>
       </c>
       <c r="B100" s="12">
@@ -3732,7 +3732,7 @@
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A101" s="26">
+      <c r="A101" s="22">
         <v>91</v>
       </c>
       <c r="B101" s="12">
@@ -3761,22 +3761,22 @@
       </c>
     </row>
     <row r="102" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A102" s="23" t="s">
+      <c r="A102" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="B102" s="18"/>
-      <c r="C102" s="18"/>
-      <c r="D102" s="18"/>
-      <c r="E102" s="18"/>
-      <c r="F102" s="18"/>
-      <c r="G102" s="18" t="s">
+      <c r="B102" s="29"/>
+      <c r="C102" s="29"/>
+      <c r="D102" s="29"/>
+      <c r="E102" s="29"/>
+      <c r="F102" s="29"/>
+      <c r="G102" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="H102" s="18"/>
-      <c r="I102" s="24"/>
+      <c r="H102" s="29"/>
+      <c r="I102" s="30"/>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A103" s="26">
+      <c r="A103" s="22">
         <v>92</v>
       </c>
       <c r="B103" s="13">
@@ -3805,7 +3805,7 @@
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A104" s="26">
+      <c r="A104" s="22">
         <v>93</v>
       </c>
       <c r="B104" s="13">
@@ -3834,7 +3834,7 @@
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A105" s="26">
+      <c r="A105" s="22">
         <v>94</v>
       </c>
       <c r="B105" s="13">
@@ -3863,7 +3863,7 @@
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A106" s="26">
+      <c r="A106" s="22">
         <v>95</v>
       </c>
       <c r="B106" s="13">
@@ -3892,7 +3892,7 @@
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A107" s="26">
+      <c r="A107" s="22">
         <v>96</v>
       </c>
       <c r="B107" s="13">
@@ -3921,7 +3921,7 @@
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A108" s="26">
+      <c r="A108" s="22">
         <v>97</v>
       </c>
       <c r="B108" s="13">
@@ -3950,7 +3950,7 @@
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A109" s="26">
+      <c r="A109" s="22">
         <v>98</v>
       </c>
       <c r="B109" s="13">
@@ -3979,7 +3979,7 @@
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A110" s="26">
+      <c r="A110" s="22">
         <v>99</v>
       </c>
       <c r="B110" s="13">
@@ -4008,7 +4008,7 @@
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A111" s="26">
+      <c r="A111" s="22">
         <v>100</v>
       </c>
       <c r="B111" s="13">
@@ -4037,7 +4037,7 @@
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A112" s="26">
+      <c r="A112" s="22">
         <v>101</v>
       </c>
       <c r="B112" s="13">
@@ -4066,7 +4066,7 @@
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A113" s="26">
+      <c r="A113" s="22">
         <v>102</v>
       </c>
       <c r="B113" s="13">
@@ -4095,7 +4095,7 @@
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A114" s="26">
+      <c r="A114" s="22">
         <v>103</v>
       </c>
       <c r="B114" s="13">
@@ -4124,7 +4124,7 @@
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A115" s="26">
+      <c r="A115" s="22">
         <v>104</v>
       </c>
       <c r="B115" s="13">
@@ -4153,44 +4153,44 @@
       </c>
     </row>
     <row r="116" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A116" s="23" t="s">
+      <c r="A116" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="B116" s="18"/>
-      <c r="C116" s="18"/>
-      <c r="D116" s="18"/>
-      <c r="E116" s="18"/>
-      <c r="F116" s="18"/>
-      <c r="G116" s="18" t="s">
+      <c r="B116" s="29"/>
+      <c r="C116" s="29"/>
+      <c r="D116" s="29"/>
+      <c r="E116" s="29"/>
+      <c r="F116" s="29"/>
+      <c r="G116" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="H116" s="18"/>
-      <c r="I116" s="24"/>
+      <c r="H116" s="29"/>
+      <c r="I116" s="30"/>
     </row>
     <row r="117" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A117" s="23" t="s">
+      <c r="A117" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="B117" s="18"/>
-      <c r="C117" s="18"/>
-      <c r="D117" s="18"/>
-      <c r="E117" s="18"/>
-      <c r="F117" s="18"/>
-      <c r="G117" s="18" t="s">
+      <c r="B117" s="29"/>
+      <c r="C117" s="29"/>
+      <c r="D117" s="29"/>
+      <c r="E117" s="29"/>
+      <c r="F117" s="29"/>
+      <c r="G117" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="H117" s="18"/>
-      <c r="I117" s="24"/>
+      <c r="H117" s="29"/>
+      <c r="I117" s="30"/>
     </row>
     <row r="118" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A118" s="27" t="s">
+      <c r="A118" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="B118" s="19" t="s">
+      <c r="B118" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="C118" s="19"/>
-      <c r="D118" s="19"/>
+      <c r="C118" s="27"/>
+      <c r="D118" s="27"/>
       <c r="E118" s="14"/>
       <c r="F118" s="14"/>
       <c r="G118" s="14"/>
@@ -4198,14 +4198,14 @@
       <c r="I118" s="15"/>
     </row>
     <row r="119" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A119" s="27" t="s">
+      <c r="A119" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="B119" s="19" t="s">
+      <c r="B119" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="C119" s="19"/>
-      <c r="D119" s="19"/>
+      <c r="C119" s="27"/>
+      <c r="D119" s="27"/>
       <c r="E119" s="14"/>
       <c r="F119" s="14"/>
       <c r="G119" s="14"/>
@@ -4213,14 +4213,14 @@
       <c r="I119" s="15"/>
     </row>
     <row r="120" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A120" s="27" t="s">
+      <c r="A120" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="B120" s="19" t="s">
+      <c r="B120" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="C120" s="19"/>
-      <c r="D120" s="19"/>
+      <c r="C120" s="27"/>
+      <c r="D120" s="27"/>
       <c r="E120" s="14"/>
       <c r="F120" s="14"/>
       <c r="G120" s="14"/>
@@ -4228,14 +4228,14 @@
       <c r="I120" s="15"/>
     </row>
     <row r="121" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A121" s="27" t="s">
+      <c r="A121" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="B121" s="19" t="s">
+      <c r="B121" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="C121" s="19"/>
-      <c r="D121" s="19"/>
+      <c r="C121" s="27"/>
+      <c r="D121" s="27"/>
       <c r="E121" s="14"/>
       <c r="F121" s="14"/>
       <c r="G121" s="14"/>
@@ -4243,14 +4243,14 @@
       <c r="I121" s="15"/>
     </row>
     <row r="122" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A122" s="27" t="s">
+      <c r="A122" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="B122" s="19" t="s">
+      <c r="B122" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="C122" s="19"/>
-      <c r="D122" s="19"/>
+      <c r="C122" s="27"/>
+      <c r="D122" s="27"/>
       <c r="E122" s="14"/>
       <c r="F122" s="14"/>
       <c r="G122" s="14"/>
@@ -4258,19 +4258,19 @@
       <c r="I122" s="15"/>
     </row>
     <row r="123" spans="1:9" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A123" s="28" t="s">
+      <c r="A123" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="B123" s="29"/>
-      <c r="C123" s="29"/>
-      <c r="D123" s="29"/>
-      <c r="E123" s="29"/>
-      <c r="F123" s="29"/>
-      <c r="G123" s="29" t="s">
+      <c r="B123" s="25"/>
+      <c r="C123" s="25"/>
+      <c r="D123" s="25"/>
+      <c r="E123" s="25"/>
+      <c r="F123" s="25"/>
+      <c r="G123" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="H123" s="29"/>
-      <c r="I123" s="30"/>
+      <c r="H123" s="25"/>
+      <c r="I123" s="26"/>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D124" s="16"/>
@@ -4326,6 +4326,30 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="A25:F25"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="A34:F34"/>
+    <mergeCell ref="G34:I34"/>
+    <mergeCell ref="A47:F47"/>
+    <mergeCell ref="G47:I47"/>
+    <mergeCell ref="A59:F59"/>
+    <mergeCell ref="G59:I59"/>
+    <mergeCell ref="A68:F68"/>
+    <mergeCell ref="G68:I68"/>
+    <mergeCell ref="A79:F79"/>
+    <mergeCell ref="G79:I79"/>
+    <mergeCell ref="A90:F90"/>
+    <mergeCell ref="G90:I90"/>
+    <mergeCell ref="A102:F102"/>
+    <mergeCell ref="G102:I102"/>
+    <mergeCell ref="A116:F116"/>
+    <mergeCell ref="G116:I116"/>
+    <mergeCell ref="A117:F117"/>
+    <mergeCell ref="G117:I117"/>
     <mergeCell ref="A123:F123"/>
     <mergeCell ref="G123:I123"/>
     <mergeCell ref="B118:D118"/>
@@ -4333,30 +4357,6 @@
     <mergeCell ref="B120:D120"/>
     <mergeCell ref="B121:D121"/>
     <mergeCell ref="B122:D122"/>
-    <mergeCell ref="A102:F102"/>
-    <mergeCell ref="G102:I102"/>
-    <mergeCell ref="A116:F116"/>
-    <mergeCell ref="G116:I116"/>
-    <mergeCell ref="A117:F117"/>
-    <mergeCell ref="G117:I117"/>
-    <mergeCell ref="A68:F68"/>
-    <mergeCell ref="G68:I68"/>
-    <mergeCell ref="A79:F79"/>
-    <mergeCell ref="G79:I79"/>
-    <mergeCell ref="A90:F90"/>
-    <mergeCell ref="G90:I90"/>
-    <mergeCell ref="A34:F34"/>
-    <mergeCell ref="G34:I34"/>
-    <mergeCell ref="A47:F47"/>
-    <mergeCell ref="G47:I47"/>
-    <mergeCell ref="A59:F59"/>
-    <mergeCell ref="G59:I59"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="A13:F13"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="A25:F25"/>
-    <mergeCell ref="G25:I25"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>